<commit_message>
Design and music and stuff
</commit_message>
<xml_diff>
--- a/assets/Credits.xlsx
+++ b/assets/Credits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spec\Documents\GitHub\TowerDefense\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87FA8EE-9083-4FE0-B557-011FE5A76FD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{173C6011-6332-4434-BEDD-56C99C8DE6FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9810" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,51 +32,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Delapouite</t>
+    <t>Intro</t>
   </si>
   <si>
-    <t>https://game-icons.net/1x1/delapouite/frozen-ring.html</t>
+    <t>https://opengameart.org/content/baroque-opusendo</t>
   </si>
   <si>
-    <t>https://game-icons.net/1x1/delapouite/evil-love.html</t>
-  </si>
-  <si>
-    <t>Demonologist</t>
-  </si>
-  <si>
-    <t>Lucifer</t>
-  </si>
-  <si>
-    <t>Skoll</t>
-  </si>
-  <si>
-    <t>https://game-icons.net/1x1/skoll/fangs.html</t>
-  </si>
-  <si>
-    <t>Bloodhound</t>
-  </si>
-  <si>
-    <t>https://game-icons.net/1x1/delapouite/woman-elf-face.html</t>
-  </si>
-  <si>
-    <t>Elven</t>
-  </si>
-  <si>
-    <t>Lorc</t>
-  </si>
-  <si>
-    <t>https://game-icons.net/1x1/lorc/death-zone.html</t>
-  </si>
-  <si>
-    <t>Death Knight</t>
-  </si>
-  <si>
-    <t>https://game-icons.net/1x1/lorc/sharped-teeth-skull.html</t>
-  </si>
-  <si>
-    <t>https://game-icons.net/1x1/lorc/batwing-emblem.html</t>
+    <t>Baroque Opusendo</t>
   </si>
 </sst>
 </file>
@@ -407,13 +372,14 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -424,66 +390,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{ABB6B130-DBAE-4FF5-8960-A171EDA0C82F}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F5D3C1B7-9F1E-4FFE-BC69-B999D9A24D69}"/>
-    <hyperlink ref="B20" r:id="rId3" xr:uid="{87B2BDCA-F07D-46AA-A479-80158D08888D}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{2BA39EA9-1DDF-4FA6-AEF2-7BA3F7EEFC89}"/>
-    <hyperlink ref="B30" r:id="rId5" xr:uid="{D815E688-353A-447E-AAD3-D5166EAF5217}"/>
-    <hyperlink ref="B31" r:id="rId6" xr:uid="{ACF5A7CE-019C-466F-8C3D-F31A19788FCF}"/>
-    <hyperlink ref="B32" r:id="rId7" xr:uid="{1F5E7054-BB31-42EA-AE2A-1DED2E442125}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{382A3497-1BB8-4E89-8205-74EDDE7EE6F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>